<commit_message>
Mise à jour du fichier des couleurs
</commit_message>
<xml_diff>
--- a/Ressources/Couleurs.xlsx
+++ b/Ressources/Couleurs.xlsx
@@ -48,10 +48,10 @@
     <t>#f9a01b</t>
   </si>
   <si>
-    <t>#005dac</t>
-  </si>
-  <si>
     <t>#0097dc</t>
+  </si>
+  <si>
+    <t>#083a7c</t>
   </si>
 </sst>
 </file>
@@ -88,13 +88,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF005DDC"/>
+        <fgColor rgb="FF0097DC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0097DC"/>
+        <fgColor rgb="FF083A7C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -152,6 +152,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF083A7C"/>
       <color rgb="FF0097DC"/>
       <color rgb="FF005DDC"/>
       <color rgb="FFF9A01B"/>
@@ -434,7 +435,7 @@
   <dimension ref="B2:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,18 +485,18 @@
         <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1">
-        <v>93</v>
+        <v>58</v>
       </c>
       <c r="E4" s="1">
-        <v>172</v>
+        <v>124</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
@@ -511,9 +512,9 @@
         <v>220</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="6"/>
+        <v>9</v>
+      </c>
+      <c r="G5" s="5"/>
     </row>
     <row r="6" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>

</xml_diff>